<commit_message>
update the previous version
</commit_message>
<xml_diff>
--- a/Slickdeals_Test_Case_Project/Slickdeals_Test_Case.xlsx
+++ b/Slickdeals_Test_Case_Project/Slickdeals_Test_Case.xlsx
@@ -4,6 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="TestCase" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Report" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Test Matrix" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Bug Report" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Remember_Me_checkbox_error">TestCase!$J$17</definedName>
@@ -13,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="387">
   <si>
     <t>Product Name</t>
   </si>
@@ -1068,6 +1071,1119 @@
   <si>
     <t>Back Button Error</t>
   </si>
+  <si>
+    <t>Test Case Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Project Name   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module Name   </t>
+  </si>
+  <si>
+    <t>Sign Up and Sign In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total No. </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Result :</t>
+  </si>
+  <si>
+    <t>Test Case Version</t>
+  </si>
+  <si>
+    <t>Written By</t>
+  </si>
+  <si>
+    <t>Executed By</t>
+  </si>
+  <si>
+    <t>New Features</t>
+  </si>
+  <si>
+    <t>Testing Scope</t>
+  </si>
+  <si>
+    <t>Testing Environment :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Chrome Browser </t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>TEST EXECUTION REPORT</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Out Of Scope</t>
+  </si>
+  <si>
+    <t>Total TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total  </t>
+  </si>
+  <si>
+    <t>LIMITATIONS</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received </t>
+  </si>
+  <si>
+    <t>Useful</t>
+  </si>
+  <si>
+    <t>PRD</t>
+  </si>
+  <si>
+    <t>USER STORY</t>
+  </si>
+  <si>
+    <t>Testing Type
+in Scope</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Yes/ No.
+Justification (If No):</t>
+  </si>
+  <si>
+    <t>This type of testing ignores the internal parts and focuses only on the output to check if it is as per the requirement or not.</t>
+  </si>
+  <si>
+    <t>Integration Testing</t>
+  </si>
+  <si>
+    <t>Testing of all integrated modules to verify the combined functionality after integration is termed as Integration Testing.</t>
+  </si>
+  <si>
+    <t>Negative Testing</t>
+  </si>
+  <si>
+    <t>Testing having the mindset of “attitude to break” using incorrect data and invalid inputs.</t>
+  </si>
+  <si>
+    <t>Usability Testing</t>
+  </si>
+  <si>
+    <t>Test application from user friendliness perspective.</t>
+  </si>
+  <si>
+    <t>Browser Compatibility Testing</t>
+  </si>
+  <si>
+    <t>Browser Compatibility Testing is performed for web applications and it ensures that the software can run with the combination of different browser and operating system. This type of testing also validates whether web application runs on all versions of all browsers or not.</t>
+  </si>
+  <si>
+    <t>Boundary Value Testing</t>
+  </si>
+  <si>
+    <t>There is an upper and lower boundary for each range and testing is performed on these boundary values.</t>
+  </si>
+  <si>
+    <t>Risk Based Testing
+Or
+Regression Testing</t>
+  </si>
+  <si>
+    <t>Risk-Based Testing includes testing of highly critical functionality, which has the highest impact on business and in which the probability of failure is very high.
+Testing an application as a whole for the modification in any module or functionality is termed as Regression Testing.</t>
+  </si>
+  <si>
+    <t>Test Metrics</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Result (%)</t>
+  </si>
+  <si>
+    <t>Percentage of Test Cases Executed</t>
+  </si>
+  <si>
+    <t>(No. of Test Cases Executed / Total no. of Test Cases Written) * 100</t>
+  </si>
+  <si>
+    <t>(66/66)*100 = 100</t>
+  </si>
+  <si>
+    <t>Percentage of Test Cases Not Executed</t>
+  </si>
+  <si>
+    <t>(No. of Test Cases not Executed / Total no. of Test Cases Written) * 100</t>
+  </si>
+  <si>
+    <t>(0/66)*100 = 0</t>
+  </si>
+  <si>
+    <t>Percentage of Test Cases Passed</t>
+  </si>
+  <si>
+    <t>(No. of Test Cases Passed / Total no. of Test Cases Executed) * 100</t>
+  </si>
+  <si>
+    <t>(58/66)*100 = 87.87</t>
+  </si>
+  <si>
+    <t>Percentage of Test Cases Failed</t>
+  </si>
+  <si>
+    <t>(No. of Test Cases Failed / Total no. of Test Cases Executed) * 100</t>
+  </si>
+  <si>
+    <t>(8/66)*100 = 12.12</t>
+  </si>
+  <si>
+    <t>Percentage of Test Cases Blocked</t>
+  </si>
+  <si>
+    <t>(No. of Test Cases Blocked / Total no. of Test Cases Executed) * 100</t>
+  </si>
+  <si>
+    <t>Defect Density</t>
+  </si>
+  <si>
+    <t>No. of Defects found / Size (No. of Requirements)</t>
+  </si>
+  <si>
+    <t>Defect Removal Efficiency (DRE)</t>
+  </si>
+  <si>
+    <t>(Fixed Defects / (Fixed Defects + Missed Defects)) * 100</t>
+  </si>
+  <si>
+    <t>Defect Leakage</t>
+  </si>
+  <si>
+    <t>(No. of Defects found in UAT/ No. of Defects found in Testing) * 100</t>
+  </si>
+  <si>
+    <t>Defect Rejection Ratio</t>
+  </si>
+  <si>
+    <t>(No. of Defects Rejected/ Total no. of Defects Raised) * 100</t>
+  </si>
+  <si>
+    <t>Defect Age</t>
+  </si>
+  <si>
+    <t>Fixed date - Reported date</t>
+  </si>
+  <si>
+    <t>Customer Satisfaction</t>
+  </si>
+  <si>
+    <t>No. of complaints per Period of Time</t>
+  </si>
+  <si>
+    <t>Bug Reporting</t>
+  </si>
+  <si>
+    <t># SL 07</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Issue: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">placeholder text for input fields is visible </t>
+    </r>
+  </si>
+  <si>
+    <t>Reproducing Steps:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Module: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Sign Up</t>
+    </r>
+  </si>
+  <si>
+    <t>Severity:low</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Priority:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> low</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Your email address placeholder text missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Issue:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> CAPTCHA popup appear beneat the registration page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Module: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Sign Up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Medium</t>
+    </r>
+  </si>
+  <si>
+    <t>Priority:  High</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>CAPTCHA popup error</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 30</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Issue: user can</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> register using common email mistakes</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner
+3.Enter invalid uncommon email formats then click "Continue" button</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Module: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t>Sign Up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">  Low</t>
+    </r>
+  </si>
+  <si>
+    <t>Priority: Medium</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>invalid email</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF0000FF"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 35</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Issue:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> "Back" button does not reset the form fields</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner
+3.Click "Back" to return to the previous screen then  enter valid email the click "Continue" button then check all the input fields</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Module: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Sign Up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> P1</t>
+    </r>
+  </si>
+  <si>
+    <t>Priority: p4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Back button error</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 54</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Issue: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> invalid email format</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner then click on Log In button
+3.Enter invalid email address then click the "Continue" button.</t>
+  </si>
+  <si>
+    <t>Module: Log In</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> P1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Invalid email address</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 55</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Issue: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">invalid user name </t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner then click on Log In button
+3.Enter invalid user name then click the "Continue" button.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> P1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Invalid user name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 60</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Issue: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>password with fewer than 8 characters</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner then click on Log In button
+3.Enter valid email address or user name then click the "Continue" button. Then enter a password with fewer than 8 character then check "Log In" button</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> P1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Password with fewer than 8 characters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
+  <si>
+    <t># SL 66</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Issue: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> "Back" button does not reset the password field</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Go to the URL
+   https://slickdeals.net/
+2. Click on Log In/Sign Up button at the right corner then click on Log In button
+3.Enter valid email address or user name then click the "Continue" button. Then enter a valid password.Then click the back"&lt;" button then again enter valid email address or user name then click the "Continue" button then check the password field</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Severity:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> P1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">Screenshot: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>Back Button Error</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Responsible QA:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Khaled Hasan</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1076,7 +2192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="41">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1231,8 +2347,73 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Comfortaa"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1311,8 +2492,116 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0070C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DBDB"/>
+        <bgColor rgb="FFF2DBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6DDE8"/>
+        <bgColor rgb="FFB6DDE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FFDBE5F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
+        <bgColor rgb="FF99FF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0D9"/>
+        <bgColor rgb="FFCCC0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFABF8F"/>
+        <bgColor rgb="FFFABF8F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5B8B7"/>
+        <bgColor rgb="FFE5B8B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC2D69B"/>
+        <bgColor rgb="FFC2D69B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAF1DD"/>
+        <bgColor rgb="FFEAF1DD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2A1C7"/>
+        <bgColor rgb="FFB2A1C7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95B3D7"/>
+        <bgColor rgb="FF95B3D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="48">
     <border/>
     <border>
       <left style="medium">
@@ -1551,11 +2840,220 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+    </border>
+    <border>
+      <top/>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="194">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1746,7 +3244,7 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="14" fillId="10" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1888,6 +3386,201 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="14" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="23" fillId="15" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="24" fillId="16" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="27" fillId="15" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="24" fillId="16" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="17" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="24" fillId="16" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="28" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="29" fillId="10" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="30" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="24" fillId="16" fontId="29" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="31" fillId="18" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="35" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="19" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="36" fillId="19" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="37" fillId="19" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="23" fillId="20" fontId="29" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="36" fillId="21" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="36" fillId="22" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="36" fillId="23" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="36" fillId="24" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="37" fillId="25" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="27" fillId="26" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="38" fillId="26" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="38" fillId="26" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="26" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="27" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="27" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="27" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="27" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="28" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="14" fillId="28" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="28" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="29" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="15" fillId="29" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="39" fillId="29" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="41" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="39" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="39" fillId="30" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="14" fillId="18" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="42" fillId="18" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="38" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="29" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="39" fillId="25" fontId="39" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="41" fillId="31" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="31" fillId="31" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="43" fillId="31" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="44" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="43" fillId="31" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="43" fillId="31" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="43" fillId="31" fontId="29" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="43" fillId="31" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="43" fillId="31" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="45" fillId="31" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="46" fillId="31" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="47" fillId="31" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1939,6 +3632,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -5749,4 +7454,2536 @@
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="8.57"/>
+    <col customWidth="1" min="4" max="4" width="0.43"/>
+    <col customWidth="1" min="6" max="6" width="18.14"/>
+    <col customWidth="1" min="18" max="18" width="25.29"/>
+  </cols>
+  <sheetData>
+    <row r="21">
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="117"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="117"/>
+      <c r="L21" s="117"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="117"/>
+      <c r="O21" s="117"/>
+      <c r="P21" s="117"/>
+      <c r="Q21" s="117"/>
+      <c r="R21" s="117"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="117"/>
+      <c r="N22" s="117"/>
+      <c r="O22" s="117"/>
+      <c r="P22" s="117"/>
+      <c r="Q22" s="117"/>
+      <c r="R22" s="117"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="117"/>
+      <c r="O23" s="117"/>
+      <c r="P23" s="117"/>
+      <c r="Q23" s="117"/>
+      <c r="R23" s="117"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="117"/>
+      <c r="E24" s="118" t="s">
+        <v>259</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="117"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="117"/>
+      <c r="P24" s="117"/>
+      <c r="Q24" s="117"/>
+      <c r="R24" s="117"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="117"/>
+      <c r="E25" s="119" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" s="120" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="117"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="117"/>
+      <c r="N25" s="117"/>
+      <c r="O25" s="117"/>
+      <c r="P25" s="117"/>
+      <c r="Q25" s="117"/>
+      <c r="R25" s="117"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="117"/>
+      <c r="E26" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="F26" s="124" t="s">
+        <v>262</v>
+      </c>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="117"/>
+      <c r="L26" s="125" t="s">
+        <v>263</v>
+      </c>
+      <c r="M26" s="125" t="s">
+        <v>264</v>
+      </c>
+      <c r="N26" s="117"/>
+      <c r="O26" s="126" t="s">
+        <v>265</v>
+      </c>
+      <c r="P26" s="117"/>
+      <c r="Q26" s="117"/>
+      <c r="R26" s="117"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="117"/>
+      <c r="E27" s="119" t="s">
+        <v>266</v>
+      </c>
+      <c r="F27" s="127">
+        <v>1.0</v>
+      </c>
+      <c r="G27" s="121"/>
+      <c r="H27" s="121"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="128">
+        <f>F35</f>
+        <v>58</v>
+      </c>
+      <c r="M27" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="129"/>
+      <c r="O27" s="130"/>
+      <c r="P27" s="117"/>
+      <c r="Q27" s="117"/>
+      <c r="R27" s="117"/>
+    </row>
+    <row r="28">
+      <c r="D28" s="117"/>
+      <c r="E28" s="119" t="s">
+        <v>267</v>
+      </c>
+      <c r="F28" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="128">
+        <f>G35</f>
+        <v>8</v>
+      </c>
+      <c r="M28" s="128" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="129"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="117"/>
+      <c r="Q28" s="117"/>
+      <c r="R28" s="117"/>
+    </row>
+    <row r="29">
+      <c r="D29" s="117"/>
+      <c r="E29" s="119" t="s">
+        <v>268</v>
+      </c>
+      <c r="F29" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="121"/>
+      <c r="H29" s="121"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="117"/>
+      <c r="L29" s="128">
+        <f>H35</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="128" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29" s="117"/>
+      <c r="O29" s="132" t="s">
+        <v>269</v>
+      </c>
+      <c r="P29" s="133" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q29" s="133" t="s">
+        <v>271</v>
+      </c>
+      <c r="R29" s="134" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" s="117"/>
+      <c r="E30" s="119" t="s">
+        <v>273</v>
+      </c>
+      <c r="F30" s="135"/>
+      <c r="G30" s="121"/>
+      <c r="H30" s="121"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="117"/>
+      <c r="L30" s="128">
+        <f>I35</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="128" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="117"/>
+      <c r="O30" s="130"/>
+      <c r="P30" s="130"/>
+      <c r="Q30" s="130"/>
+      <c r="R30" s="130"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="117"/>
+      <c r="E31" s="136" t="s">
+        <v>274</v>
+      </c>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="137"/>
+      <c r="J31" s="138"/>
+      <c r="K31" s="117"/>
+      <c r="L31" s="117"/>
+      <c r="M31" s="117"/>
+      <c r="N31" s="117"/>
+      <c r="O31" s="117"/>
+      <c r="P31" s="117"/>
+      <c r="Q31" s="117"/>
+      <c r="R31" s="117"/>
+    </row>
+    <row r="32">
+      <c r="D32" s="117"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="117"/>
+      <c r="L32" s="117"/>
+      <c r="M32" s="117"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="117"/>
+      <c r="P32" s="117"/>
+      <c r="Q32" s="117"/>
+      <c r="R32" s="117"/>
+    </row>
+    <row r="33">
+      <c r="D33" s="117"/>
+      <c r="E33" s="141" t="s">
+        <v>275</v>
+      </c>
+      <c r="F33" s="142" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="142" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="142" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="142" t="s">
+        <v>276</v>
+      </c>
+      <c r="J33" s="143" t="s">
+        <v>277</v>
+      </c>
+      <c r="K33" s="117"/>
+      <c r="L33" s="117"/>
+      <c r="M33" s="117"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="117"/>
+      <c r="P33" s="117"/>
+      <c r="Q33" s="117"/>
+      <c r="R33" s="117"/>
+    </row>
+    <row r="34">
+      <c r="D34" s="144"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="146">
+        <f>TestCase!M2</f>
+        <v>58</v>
+      </c>
+      <c r="G34" s="147">
+        <f>TestCase!M3</f>
+        <v>8</v>
+      </c>
+      <c r="H34" s="148" t="str">
+        <f>TestCase!P24</f>
+        <v/>
+      </c>
+      <c r="I34" s="149" t="str">
+        <f>TestCase!P25</f>
+        <v/>
+      </c>
+      <c r="J34" s="150" t="str">
+        <f>TestCase!P26</f>
+        <v/>
+      </c>
+      <c r="K34" s="144"/>
+      <c r="L34" s="144"/>
+      <c r="M34" s="144"/>
+      <c r="N34" s="144"/>
+      <c r="O34" s="144"/>
+      <c r="P34" s="144"/>
+      <c r="Q34" s="144"/>
+      <c r="R34" s="144"/>
+    </row>
+    <row r="35">
+      <c r="D35" s="117"/>
+      <c r="E35" s="151" t="s">
+        <v>278</v>
+      </c>
+      <c r="F35" s="152">
+        <f t="shared" ref="F35:J35" si="1">SUM(F34)</f>
+        <v>58</v>
+      </c>
+      <c r="G35" s="153">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H35" s="152">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="152">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="154">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="117"/>
+      <c r="N35" s="117"/>
+      <c r="O35" s="117"/>
+      <c r="P35" s="117"/>
+      <c r="Q35" s="117"/>
+      <c r="R35" s="117"/>
+    </row>
+    <row r="36">
+      <c r="D36" s="117"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
+      <c r="H36" s="155"/>
+      <c r="I36" s="155"/>
+      <c r="J36" s="155"/>
+      <c r="K36" s="117"/>
+      <c r="L36" s="117"/>
+      <c r="M36" s="117"/>
+      <c r="N36" s="117"/>
+      <c r="O36" s="117"/>
+      <c r="P36" s="117"/>
+      <c r="Q36" s="117"/>
+      <c r="R36" s="117"/>
+    </row>
+    <row r="37">
+      <c r="D37" s="117"/>
+      <c r="E37" s="155"/>
+      <c r="F37" s="155"/>
+      <c r="G37" s="155"/>
+      <c r="H37" s="155"/>
+      <c r="I37" s="155"/>
+      <c r="J37" s="155"/>
+      <c r="K37" s="117"/>
+      <c r="L37" s="117"/>
+      <c r="M37" s="117"/>
+      <c r="N37" s="117"/>
+      <c r="O37" s="117"/>
+      <c r="P37" s="117"/>
+      <c r="Q37" s="117"/>
+      <c r="R37" s="117"/>
+    </row>
+    <row r="38">
+      <c r="D38" s="117"/>
+      <c r="E38" s="156" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="117"/>
+      <c r="L38" s="117"/>
+      <c r="M38" s="117"/>
+      <c r="N38" s="117"/>
+      <c r="O38" s="117"/>
+      <c r="P38" s="117"/>
+      <c r="Q38" s="117"/>
+      <c r="R38" s="117"/>
+    </row>
+    <row r="39">
+      <c r="D39" s="117"/>
+      <c r="E39" s="157" t="s">
+        <v>280</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="158"/>
+      <c r="I39" s="159" t="s">
+        <v>281</v>
+      </c>
+      <c r="J39" s="159" t="s">
+        <v>282</v>
+      </c>
+      <c r="K39" s="117"/>
+      <c r="L39" s="117"/>
+      <c r="M39" s="117"/>
+      <c r="N39" s="117"/>
+      <c r="O39" s="117"/>
+      <c r="P39" s="117"/>
+      <c r="Q39" s="117"/>
+      <c r="R39" s="117"/>
+    </row>
+    <row r="40">
+      <c r="D40" s="117"/>
+      <c r="E40" s="160" t="s">
+        <v>283</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="161"/>
+      <c r="I40" s="162" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="162" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="117"/>
+      <c r="L40" s="117"/>
+      <c r="M40" s="117"/>
+      <c r="N40" s="117"/>
+      <c r="O40" s="117"/>
+      <c r="P40" s="117"/>
+      <c r="Q40" s="117"/>
+      <c r="R40" s="117"/>
+    </row>
+    <row r="41">
+      <c r="D41" s="117"/>
+      <c r="E41" s="160" t="s">
+        <v>284</v>
+      </c>
+      <c r="F41" s="24"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="161"/>
+      <c r="I41" s="162" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="162" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="117"/>
+      <c r="L41" s="117"/>
+      <c r="M41" s="117"/>
+      <c r="N41" s="117"/>
+      <c r="O41" s="117"/>
+      <c r="P41" s="117"/>
+      <c r="Q41" s="117"/>
+      <c r="R41" s="117"/>
+    </row>
+    <row r="42">
+      <c r="D42" s="117"/>
+      <c r="E42" s="117"/>
+      <c r="F42" s="117"/>
+      <c r="G42" s="117"/>
+      <c r="H42" s="117"/>
+      <c r="I42" s="117"/>
+      <c r="J42" s="117"/>
+      <c r="K42" s="117"/>
+      <c r="L42" s="117"/>
+      <c r="M42" s="117"/>
+      <c r="N42" s="117"/>
+      <c r="O42" s="117"/>
+      <c r="P42" s="117"/>
+      <c r="Q42" s="117"/>
+      <c r="R42" s="117"/>
+    </row>
+    <row r="43">
+      <c r="D43" s="117"/>
+      <c r="E43" s="163"/>
+      <c r="F43" s="164" t="s">
+        <v>285</v>
+      </c>
+      <c r="G43" s="165" t="s">
+        <v>286</v>
+      </c>
+      <c r="H43" s="166"/>
+      <c r="I43" s="166"/>
+      <c r="J43" s="167"/>
+      <c r="K43" s="117"/>
+      <c r="L43" s="117"/>
+      <c r="M43" s="117"/>
+      <c r="N43" s="117"/>
+      <c r="O43" s="117"/>
+      <c r="P43" s="117"/>
+      <c r="Q43" s="117"/>
+      <c r="R43" s="117"/>
+    </row>
+    <row r="44">
+      <c r="D44" s="117"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="168"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="117"/>
+      <c r="L44" s="117"/>
+      <c r="M44" s="117"/>
+      <c r="N44" s="117"/>
+      <c r="O44" s="117"/>
+      <c r="P44" s="117"/>
+      <c r="Q44" s="117"/>
+      <c r="R44" s="117"/>
+    </row>
+    <row r="45">
+      <c r="D45" s="117"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="168"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="117"/>
+      <c r="L45" s="117"/>
+      <c r="M45" s="117"/>
+      <c r="N45" s="117"/>
+      <c r="O45" s="117"/>
+      <c r="P45" s="117"/>
+      <c r="Q45" s="117"/>
+      <c r="R45" s="117"/>
+    </row>
+    <row r="46">
+      <c r="D46" s="117"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="139"/>
+      <c r="H46" s="140"/>
+      <c r="I46" s="140"/>
+      <c r="J46" s="72"/>
+      <c r="K46" s="117"/>
+      <c r="L46" s="117"/>
+      <c r="M46" s="117"/>
+      <c r="N46" s="117"/>
+      <c r="O46" s="117"/>
+      <c r="P46" s="117"/>
+      <c r="Q46" s="117"/>
+      <c r="R46" s="117"/>
+    </row>
+    <row r="47">
+      <c r="D47" s="117"/>
+      <c r="E47" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F47" s="170" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47" s="171" t="s">
+        <v>288</v>
+      </c>
+      <c r="H47" s="166"/>
+      <c r="I47" s="166"/>
+      <c r="J47" s="167"/>
+      <c r="K47" s="117"/>
+      <c r="L47" s="117"/>
+      <c r="M47" s="117"/>
+      <c r="N47" s="117"/>
+      <c r="O47" s="117"/>
+      <c r="P47" s="117"/>
+      <c r="Q47" s="117"/>
+      <c r="R47" s="117"/>
+    </row>
+    <row r="48">
+      <c r="D48" s="117"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="168"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="117"/>
+      <c r="L48" s="117"/>
+      <c r="M48" s="117"/>
+      <c r="N48" s="117"/>
+      <c r="O48" s="117"/>
+      <c r="P48" s="117"/>
+      <c r="Q48" s="117"/>
+      <c r="R48" s="117"/>
+    </row>
+    <row r="49">
+      <c r="D49" s="117"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="168"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="117"/>
+      <c r="L49" s="117"/>
+      <c r="M49" s="117"/>
+      <c r="N49" s="117"/>
+      <c r="O49" s="117"/>
+      <c r="P49" s="117"/>
+      <c r="Q49" s="117"/>
+      <c r="R49" s="117"/>
+    </row>
+    <row r="50">
+      <c r="D50" s="117"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="139"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="140"/>
+      <c r="J50" s="72"/>
+      <c r="K50" s="117"/>
+      <c r="L50" s="117"/>
+      <c r="M50" s="117"/>
+      <c r="N50" s="117"/>
+      <c r="O50" s="117"/>
+      <c r="P50" s="117"/>
+      <c r="Q50" s="117"/>
+      <c r="R50" s="117"/>
+    </row>
+    <row r="51">
+      <c r="D51" s="117"/>
+      <c r="E51" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F51" s="170" t="s">
+        <v>289</v>
+      </c>
+      <c r="G51" s="171" t="s">
+        <v>290</v>
+      </c>
+      <c r="H51" s="166"/>
+      <c r="I51" s="166"/>
+      <c r="J51" s="167"/>
+      <c r="K51" s="117"/>
+      <c r="L51" s="117"/>
+      <c r="M51" s="117"/>
+      <c r="N51" s="117"/>
+      <c r="O51" s="117"/>
+      <c r="P51" s="117"/>
+      <c r="Q51" s="117"/>
+      <c r="R51" s="117"/>
+    </row>
+    <row r="52">
+      <c r="D52" s="117"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="168"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="117"/>
+      <c r="L52" s="117"/>
+      <c r="M52" s="117"/>
+      <c r="N52" s="117"/>
+      <c r="O52" s="117"/>
+      <c r="P52" s="117"/>
+      <c r="Q52" s="117"/>
+      <c r="R52" s="117"/>
+    </row>
+    <row r="53">
+      <c r="D53" s="117"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="63"/>
+      <c r="G53" s="168"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="117"/>
+      <c r="L53" s="117"/>
+      <c r="M53" s="117"/>
+      <c r="N53" s="117"/>
+      <c r="O53" s="117"/>
+      <c r="P53" s="117"/>
+      <c r="Q53" s="117"/>
+      <c r="R53" s="117"/>
+    </row>
+    <row r="54">
+      <c r="D54" s="117"/>
+      <c r="E54" s="96"/>
+      <c r="F54" s="96"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="140"/>
+      <c r="I54" s="140"/>
+      <c r="J54" s="72"/>
+      <c r="K54" s="117"/>
+      <c r="L54" s="117"/>
+      <c r="M54" s="117"/>
+      <c r="N54" s="117"/>
+      <c r="O54" s="117"/>
+      <c r="P54" s="117"/>
+      <c r="Q54" s="117"/>
+      <c r="R54" s="117"/>
+    </row>
+    <row r="55">
+      <c r="D55" s="117"/>
+      <c r="E55" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F55" s="170" t="s">
+        <v>291</v>
+      </c>
+      <c r="G55" s="171" t="s">
+        <v>292</v>
+      </c>
+      <c r="H55" s="166"/>
+      <c r="I55" s="166"/>
+      <c r="J55" s="167"/>
+      <c r="K55" s="117"/>
+      <c r="L55" s="117"/>
+      <c r="M55" s="117"/>
+      <c r="N55" s="117"/>
+      <c r="O55" s="117"/>
+      <c r="P55" s="117"/>
+      <c r="Q55" s="117"/>
+      <c r="R55" s="117"/>
+    </row>
+    <row r="56">
+      <c r="D56" s="117"/>
+      <c r="E56" s="63"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="168"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="117"/>
+      <c r="L56" s="117"/>
+      <c r="M56" s="117"/>
+      <c r="N56" s="117"/>
+      <c r="O56" s="117"/>
+      <c r="P56" s="117"/>
+      <c r="Q56" s="117"/>
+      <c r="R56" s="117"/>
+    </row>
+    <row r="57">
+      <c r="D57" s="117"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="168"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="117"/>
+      <c r="L57" s="117"/>
+      <c r="M57" s="117"/>
+      <c r="N57" s="117"/>
+      <c r="O57" s="117"/>
+      <c r="P57" s="117"/>
+      <c r="Q57" s="117"/>
+      <c r="R57" s="117"/>
+    </row>
+    <row r="58">
+      <c r="D58" s="117"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="96"/>
+      <c r="G58" s="139"/>
+      <c r="H58" s="140"/>
+      <c r="I58" s="140"/>
+      <c r="J58" s="72"/>
+      <c r="K58" s="117"/>
+      <c r="L58" s="117"/>
+      <c r="M58" s="117"/>
+      <c r="N58" s="117"/>
+      <c r="O58" s="117"/>
+      <c r="P58" s="117"/>
+      <c r="Q58" s="117"/>
+      <c r="R58" s="117"/>
+    </row>
+    <row r="59">
+      <c r="D59" s="117"/>
+      <c r="E59" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F59" s="170" t="s">
+        <v>293</v>
+      </c>
+      <c r="G59" s="171" t="s">
+        <v>294</v>
+      </c>
+      <c r="H59" s="166"/>
+      <c r="I59" s="166"/>
+      <c r="J59" s="167"/>
+      <c r="K59" s="117"/>
+      <c r="L59" s="117"/>
+      <c r="M59" s="117"/>
+      <c r="N59" s="117"/>
+      <c r="O59" s="117"/>
+      <c r="P59" s="117"/>
+      <c r="Q59" s="117"/>
+      <c r="R59" s="117"/>
+    </row>
+    <row r="60">
+      <c r="D60" s="117"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="168"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="117"/>
+      <c r="L60" s="117"/>
+      <c r="M60" s="117"/>
+      <c r="N60" s="117"/>
+      <c r="O60" s="117"/>
+      <c r="P60" s="117"/>
+      <c r="Q60" s="117"/>
+      <c r="R60" s="117"/>
+    </row>
+    <row r="61">
+      <c r="D61" s="117"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="168"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="117"/>
+      <c r="L61" s="117"/>
+      <c r="M61" s="117"/>
+      <c r="N61" s="117"/>
+      <c r="O61" s="117"/>
+      <c r="P61" s="117"/>
+      <c r="Q61" s="117"/>
+      <c r="R61" s="117"/>
+    </row>
+    <row r="62">
+      <c r="D62" s="117"/>
+      <c r="E62" s="96"/>
+      <c r="F62" s="96"/>
+      <c r="G62" s="139"/>
+      <c r="H62" s="140"/>
+      <c r="I62" s="140"/>
+      <c r="J62" s="72"/>
+      <c r="K62" s="117"/>
+      <c r="L62" s="117"/>
+      <c r="M62" s="117"/>
+      <c r="N62" s="117"/>
+      <c r="O62" s="117"/>
+      <c r="P62" s="117"/>
+      <c r="Q62" s="117"/>
+      <c r="R62" s="117"/>
+    </row>
+    <row r="63">
+      <c r="D63" s="117"/>
+      <c r="E63" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F63" s="172" t="s">
+        <v>295</v>
+      </c>
+      <c r="G63" s="171" t="s">
+        <v>296</v>
+      </c>
+      <c r="H63" s="166"/>
+      <c r="I63" s="166"/>
+      <c r="J63" s="167"/>
+      <c r="K63" s="117"/>
+      <c r="L63" s="117"/>
+      <c r="M63" s="117"/>
+      <c r="N63" s="117"/>
+      <c r="O63" s="117"/>
+      <c r="P63" s="117"/>
+      <c r="Q63" s="117"/>
+      <c r="R63" s="117"/>
+    </row>
+    <row r="64">
+      <c r="D64" s="117"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="168"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="117"/>
+      <c r="L64" s="117"/>
+      <c r="M64" s="117"/>
+      <c r="N64" s="117"/>
+      <c r="O64" s="117"/>
+      <c r="P64" s="117"/>
+      <c r="Q64" s="117"/>
+      <c r="R64" s="117"/>
+    </row>
+    <row r="65">
+      <c r="D65" s="117"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="168"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="117"/>
+      <c r="L65" s="117"/>
+      <c r="M65" s="117"/>
+      <c r="N65" s="117"/>
+      <c r="O65" s="117"/>
+      <c r="P65" s="117"/>
+      <c r="Q65" s="117"/>
+      <c r="R65" s="117"/>
+    </row>
+    <row r="66">
+      <c r="D66" s="117"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="96"/>
+      <c r="G66" s="139"/>
+      <c r="H66" s="140"/>
+      <c r="I66" s="140"/>
+      <c r="J66" s="72"/>
+      <c r="K66" s="117"/>
+      <c r="L66" s="117"/>
+      <c r="M66" s="117"/>
+      <c r="N66" s="117"/>
+      <c r="O66" s="117"/>
+      <c r="P66" s="117"/>
+      <c r="Q66" s="117"/>
+      <c r="R66" s="117"/>
+    </row>
+    <row r="67">
+      <c r="D67" s="117"/>
+      <c r="E67" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F67" s="172" t="s">
+        <v>297</v>
+      </c>
+      <c r="G67" s="171" t="s">
+        <v>298</v>
+      </c>
+      <c r="H67" s="166"/>
+      <c r="I67" s="166"/>
+      <c r="J67" s="167"/>
+      <c r="K67" s="117"/>
+      <c r="L67" s="117"/>
+      <c r="M67" s="117"/>
+      <c r="N67" s="117"/>
+      <c r="O67" s="117"/>
+      <c r="P67" s="117"/>
+      <c r="Q67" s="117"/>
+      <c r="R67" s="117"/>
+    </row>
+    <row r="68">
+      <c r="D68" s="117"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="168"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="117"/>
+      <c r="L68" s="117"/>
+      <c r="M68" s="117"/>
+      <c r="N68" s="117"/>
+      <c r="O68" s="117"/>
+      <c r="P68" s="117"/>
+      <c r="Q68" s="117"/>
+      <c r="R68" s="117"/>
+    </row>
+    <row r="69">
+      <c r="D69" s="117"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="168"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="117"/>
+      <c r="L69" s="117"/>
+      <c r="M69" s="117"/>
+      <c r="N69" s="117"/>
+      <c r="O69" s="117"/>
+      <c r="P69" s="117"/>
+      <c r="Q69" s="117"/>
+      <c r="R69" s="117"/>
+    </row>
+    <row r="70">
+      <c r="D70" s="117"/>
+      <c r="E70" s="96"/>
+      <c r="F70" s="96"/>
+      <c r="G70" s="139"/>
+      <c r="H70" s="140"/>
+      <c r="I70" s="140"/>
+      <c r="J70" s="72"/>
+      <c r="K70" s="117"/>
+      <c r="L70" s="117"/>
+      <c r="M70" s="117"/>
+      <c r="N70" s="117"/>
+      <c r="O70" s="117"/>
+      <c r="P70" s="117"/>
+      <c r="Q70" s="117"/>
+      <c r="R70" s="117"/>
+    </row>
+    <row r="71">
+      <c r="D71" s="117"/>
+      <c r="E71" s="169" t="s">
+        <v>287</v>
+      </c>
+      <c r="F71" s="172" t="s">
+        <v>299</v>
+      </c>
+      <c r="G71" s="171" t="s">
+        <v>300</v>
+      </c>
+      <c r="H71" s="166"/>
+      <c r="I71" s="166"/>
+      <c r="J71" s="167"/>
+      <c r="K71" s="117"/>
+      <c r="L71" s="117"/>
+      <c r="M71" s="117"/>
+      <c r="N71" s="117"/>
+      <c r="O71" s="117"/>
+      <c r="P71" s="117"/>
+      <c r="Q71" s="117"/>
+      <c r="R71" s="117"/>
+    </row>
+    <row r="72">
+      <c r="D72" s="117"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="168"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="117"/>
+      <c r="L72" s="117"/>
+      <c r="M72" s="117"/>
+      <c r="N72" s="117"/>
+      <c r="O72" s="117"/>
+      <c r="P72" s="117"/>
+      <c r="Q72" s="117"/>
+      <c r="R72" s="117"/>
+    </row>
+    <row r="73">
+      <c r="D73" s="117"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="168"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="117"/>
+      <c r="L73" s="117"/>
+      <c r="M73" s="117"/>
+      <c r="N73" s="117"/>
+      <c r="O73" s="117"/>
+      <c r="P73" s="117"/>
+      <c r="Q73" s="117"/>
+      <c r="R73" s="117"/>
+    </row>
+    <row r="74">
+      <c r="D74" s="117"/>
+      <c r="E74" s="96"/>
+      <c r="F74" s="96"/>
+      <c r="G74" s="139"/>
+      <c r="H74" s="140"/>
+      <c r="I74" s="140"/>
+      <c r="J74" s="72"/>
+      <c r="K74" s="117"/>
+      <c r="L74" s="117"/>
+      <c r="M74" s="117"/>
+      <c r="N74" s="117"/>
+      <c r="O74" s="117"/>
+      <c r="P74" s="117"/>
+      <c r="Q74" s="117"/>
+      <c r="R74" s="117"/>
+    </row>
+    <row r="75">
+      <c r="D75" s="117"/>
+      <c r="E75" s="117"/>
+      <c r="F75" s="117"/>
+      <c r="G75" s="117"/>
+      <c r="H75" s="117"/>
+      <c r="I75" s="117"/>
+      <c r="J75" s="117"/>
+      <c r="K75" s="117"/>
+      <c r="L75" s="117"/>
+      <c r="M75" s="117"/>
+      <c r="N75" s="117"/>
+      <c r="O75" s="117"/>
+      <c r="P75" s="117"/>
+      <c r="Q75" s="117"/>
+      <c r="R75" s="117"/>
+    </row>
+    <row r="76">
+      <c r="D76" s="117"/>
+      <c r="E76" s="117"/>
+      <c r="F76" s="117"/>
+      <c r="G76" s="117"/>
+      <c r="H76" s="117"/>
+      <c r="I76" s="117"/>
+      <c r="J76" s="117"/>
+      <c r="K76" s="117"/>
+      <c r="L76" s="117"/>
+      <c r="M76" s="117"/>
+      <c r="N76" s="117"/>
+      <c r="O76" s="117"/>
+      <c r="P76" s="117"/>
+      <c r="Q76" s="117"/>
+      <c r="R76" s="117"/>
+    </row>
+    <row r="77">
+      <c r="D77" s="117"/>
+      <c r="E77" s="117"/>
+      <c r="F77" s="117"/>
+      <c r="G77" s="117"/>
+      <c r="H77" s="117"/>
+      <c r="I77" s="117"/>
+      <c r="J77" s="117"/>
+      <c r="K77" s="117"/>
+      <c r="L77" s="117"/>
+      <c r="M77" s="117"/>
+      <c r="N77" s="117"/>
+      <c r="O77" s="117"/>
+      <c r="P77" s="117"/>
+      <c r="Q77" s="117"/>
+      <c r="R77" s="117"/>
+    </row>
+    <row r="78">
+      <c r="D78" s="117"/>
+      <c r="E78" s="117"/>
+      <c r="F78" s="117"/>
+      <c r="G78" s="117"/>
+      <c r="H78" s="117"/>
+      <c r="I78" s="117"/>
+      <c r="J78" s="117"/>
+      <c r="K78" s="117"/>
+      <c r="L78" s="117"/>
+      <c r="M78" s="117"/>
+      <c r="N78" s="117"/>
+      <c r="O78" s="117"/>
+      <c r="P78" s="117"/>
+      <c r="Q78" s="117"/>
+      <c r="R78" s="117"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="G47:J50"/>
+    <mergeCell ref="G51:J54"/>
+    <mergeCell ref="G55:J58"/>
+    <mergeCell ref="E31:J32"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:J46"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="F59:F62"/>
+    <mergeCell ref="G59:J62"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="G63:J66"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="F67:F70"/>
+    <mergeCell ref="G67:J70"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="G71:J74"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="F47:F50"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="F51:F54"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="F55:F58"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="34.0"/>
+    <col customWidth="1" min="4" max="4" width="59.57"/>
+    <col customWidth="1" min="5" max="5" width="18.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="117"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="117"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="117"/>
+      <c r="B3" s="173" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+    </row>
+    <row r="4" ht="28.5" customHeight="1">
+      <c r="A4" s="117"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+    </row>
+    <row r="5" ht="23.25" customHeight="1">
+      <c r="A5" s="174"/>
+      <c r="B5" s="175" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="176" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="176" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5" s="176" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="117"/>
+      <c r="B6" s="177">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="178" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="179" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="180" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="117"/>
+      <c r="B7" s="177">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="178" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" s="179" t="s">
+        <v>308</v>
+      </c>
+      <c r="E7" s="180" t="s">
+        <v>309</v>
+      </c>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+    </row>
+    <row r="8" ht="25.5" customHeight="1">
+      <c r="A8" s="144"/>
+      <c r="B8" s="177">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="178" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="179" t="s">
+        <v>311</v>
+      </c>
+      <c r="E8" s="180" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" s="144"/>
+      <c r="G8" s="144"/>
+    </row>
+    <row r="9" ht="25.5" customHeight="1">
+      <c r="A9" s="144"/>
+      <c r="B9" s="177">
+        <v>4.0</v>
+      </c>
+      <c r="C9" s="178" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="179" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="180" t="s">
+        <v>315</v>
+      </c>
+      <c r="F9" s="144"/>
+      <c r="G9" s="144"/>
+    </row>
+    <row r="10" ht="25.5" customHeight="1">
+      <c r="A10" s="144"/>
+      <c r="B10" s="177">
+        <v>5.0</v>
+      </c>
+      <c r="C10" s="178" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="179" t="s">
+        <v>317</v>
+      </c>
+      <c r="E10" s="180" t="s">
+        <v>309</v>
+      </c>
+      <c r="F10" s="144"/>
+      <c r="G10" s="144"/>
+    </row>
+    <row r="11" ht="25.5" customHeight="1">
+      <c r="A11" s="144"/>
+      <c r="B11" s="177">
+        <v>6.0</v>
+      </c>
+      <c r="C11" s="178" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11" s="179" t="s">
+        <v>319</v>
+      </c>
+      <c r="E11" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="144"/>
+      <c r="G11" s="144"/>
+    </row>
+    <row r="12" ht="25.5" customHeight="1">
+      <c r="A12" s="144"/>
+      <c r="B12" s="177">
+        <v>7.0</v>
+      </c>
+      <c r="C12" s="178" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="179" t="s">
+        <v>321</v>
+      </c>
+      <c r="E12" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="144"/>
+      <c r="G12" s="144"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" s="144"/>
+      <c r="B13" s="177">
+        <v>8.0</v>
+      </c>
+      <c r="C13" s="178" t="s">
+        <v>322</v>
+      </c>
+      <c r="D13" s="179" t="s">
+        <v>323</v>
+      </c>
+      <c r="E13" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="144"/>
+      <c r="G13" s="144"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" s="144"/>
+      <c r="B14" s="177">
+        <v>9.0</v>
+      </c>
+      <c r="C14" s="178" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14" s="179" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="144"/>
+      <c r="G14" s="144"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1">
+      <c r="A15" s="144"/>
+      <c r="B15" s="177">
+        <v>10.0</v>
+      </c>
+      <c r="C15" s="178" t="s">
+        <v>326</v>
+      </c>
+      <c r="D15" s="179" t="s">
+        <v>327</v>
+      </c>
+      <c r="E15" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+    </row>
+    <row r="16" ht="25.5" customHeight="1">
+      <c r="A16" s="144"/>
+      <c r="B16" s="177">
+        <v>11.0</v>
+      </c>
+      <c r="C16" s="178" t="s">
+        <v>328</v>
+      </c>
+      <c r="D16" s="179" t="s">
+        <v>329</v>
+      </c>
+      <c r="E16" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="117"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="117"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="117"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="117"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="117"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="117"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="117"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:E4"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="59.57"/>
+    <col customWidth="1" min="4" max="4" width="31.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="117"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="117"/>
+      <c r="B2" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="167"/>
+      <c r="D2" s="117"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="117"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="117"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="117"/>
+      <c r="B4" s="168"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="117"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="117"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="117"/>
+    </row>
+    <row r="6" ht="15.0" customHeight="1">
+      <c r="A6" s="117"/>
+      <c r="B6" s="182" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="62"/>
+      <c r="D6" s="117"/>
+    </row>
+    <row r="7" ht="10.5" customHeight="1">
+      <c r="A7" s="117"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="117"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="117"/>
+      <c r="B8" s="183" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="138"/>
+      <c r="D8" s="117"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="117"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="117"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="117"/>
+      <c r="B10" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="185"/>
+      <c r="D10" s="117"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="117"/>
+      <c r="B11" s="186" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="185"/>
+      <c r="D11" s="117"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="117"/>
+      <c r="B12" s="187"/>
+      <c r="C12" s="185"/>
+      <c r="D12" s="117"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="117"/>
+      <c r="B13" s="188" t="s">
+        <v>334</v>
+      </c>
+      <c r="C13" s="185"/>
+      <c r="D13" s="117"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="117"/>
+      <c r="B14" s="189" t="s">
+        <v>335</v>
+      </c>
+      <c r="C14" s="185"/>
+      <c r="D14" s="117"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="117"/>
+      <c r="B15" s="189" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15" s="185"/>
+      <c r="D15" s="117"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="117"/>
+      <c r="B16" s="190" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16" s="185"/>
+      <c r="D16" s="117"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="117"/>
+      <c r="B17" s="191" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17" s="122"/>
+      <c r="D17" s="117"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="117"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="117"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="117"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="117"/>
+      <c r="C25" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="D25" s="167"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="117"/>
+      <c r="C26" s="168"/>
+      <c r="D26" s="62"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="117"/>
+      <c r="C27" s="168"/>
+      <c r="D27" s="62"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="117"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="72"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="117"/>
+      <c r="C29" s="182" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" s="62"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="117"/>
+      <c r="C30" s="168"/>
+      <c r="D30" s="62"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="117"/>
+      <c r="C31" s="183" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" s="138"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="117"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="62"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="117"/>
+      <c r="C33" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="D33" s="185"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="117"/>
+      <c r="C34" s="186" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="185"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="117"/>
+      <c r="C35" s="187"/>
+      <c r="D35" s="185"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="117"/>
+      <c r="C36" s="188" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="185"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="117"/>
+      <c r="C37" s="192" t="s">
+        <v>342</v>
+      </c>
+      <c r="D37" s="193"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="117"/>
+      <c r="C38" s="189" t="s">
+        <v>343</v>
+      </c>
+      <c r="D38" s="185"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="117"/>
+      <c r="C39" s="190" t="s">
+        <v>344</v>
+      </c>
+      <c r="D39" s="185"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="117"/>
+      <c r="C40" s="191" t="s">
+        <v>345</v>
+      </c>
+      <c r="D40" s="122"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="117"/>
+      <c r="C41" s="117"/>
+      <c r="D41" s="117"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="117"/>
+      <c r="C42" s="117"/>
+      <c r="D42" s="117"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="117"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="117"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="117"/>
+      <c r="B50" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50" s="167"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="117"/>
+      <c r="B51" s="168"/>
+      <c r="C51" s="62"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="117"/>
+      <c r="B52" s="168"/>
+      <c r="C52" s="62"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="117"/>
+      <c r="B53" s="139"/>
+      <c r="C53" s="72"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="117"/>
+      <c r="B54" s="182" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54" s="62"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="117"/>
+      <c r="B55" s="168"/>
+      <c r="C55" s="62"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="117"/>
+      <c r="B56" s="183" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="138"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="117"/>
+      <c r="B57" s="168"/>
+      <c r="C57" s="62"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="117"/>
+      <c r="B58" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="C58" s="185"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="117"/>
+      <c r="B59" s="186" t="s">
+        <v>348</v>
+      </c>
+      <c r="C59" s="185"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="117"/>
+      <c r="B60" s="187"/>
+      <c r="C60" s="185"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="117"/>
+      <c r="B61" s="187" t="s">
+        <v>349</v>
+      </c>
+      <c r="C61" s="185"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="117"/>
+      <c r="B62" s="192" t="s">
+        <v>350</v>
+      </c>
+      <c r="C62" s="193"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="117"/>
+      <c r="B63" s="187" t="s">
+        <v>351</v>
+      </c>
+      <c r="C63" s="185"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="117"/>
+      <c r="B64" s="190" t="s">
+        <v>352</v>
+      </c>
+      <c r="C64" s="185"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="117"/>
+      <c r="B65" s="191" t="s">
+        <v>353</v>
+      </c>
+      <c r="C65" s="122"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="117"/>
+      <c r="B66" s="117"/>
+      <c r="C66" s="117"/>
+    </row>
+    <row r="72">
+      <c r="B72" s="117"/>
+      <c r="C72" s="117"/>
+      <c r="D72" s="117"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="117"/>
+      <c r="C73" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="D73" s="167"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="117"/>
+      <c r="C74" s="168"/>
+      <c r="D74" s="62"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="117"/>
+      <c r="C75" s="168"/>
+      <c r="D75" s="62"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="117"/>
+      <c r="C76" s="139"/>
+      <c r="D76" s="72"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="117"/>
+      <c r="C77" s="182" t="s">
+        <v>354</v>
+      </c>
+      <c r="D77" s="62"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="117"/>
+      <c r="C78" s="168"/>
+      <c r="D78" s="62"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="117"/>
+      <c r="C79" s="183" t="s">
+        <v>355</v>
+      </c>
+      <c r="D79" s="138"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="117"/>
+      <c r="C80" s="168"/>
+      <c r="D80" s="62"/>
+    </row>
+    <row r="81">
+      <c r="B81" s="117"/>
+      <c r="C81" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="D81" s="185"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="117"/>
+      <c r="C82" s="186" t="s">
+        <v>356</v>
+      </c>
+      <c r="D82" s="185"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="117"/>
+      <c r="C83" s="187"/>
+      <c r="D83" s="185"/>
+    </row>
+    <row r="84">
+      <c r="B84" s="117"/>
+      <c r="C84" s="188" t="s">
+        <v>357</v>
+      </c>
+      <c r="D84" s="185"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="117"/>
+      <c r="C85" s="192" t="s">
+        <v>358</v>
+      </c>
+      <c r="D85" s="193"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="117"/>
+      <c r="C86" s="187" t="s">
+        <v>359</v>
+      </c>
+      <c r="D86" s="185"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="117"/>
+      <c r="C87" s="190" t="s">
+        <v>360</v>
+      </c>
+      <c r="D87" s="185"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="117"/>
+      <c r="C88" s="191" t="s">
+        <v>361</v>
+      </c>
+      <c r="D88" s="122"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="117"/>
+      <c r="C89" s="117"/>
+      <c r="D89" s="117"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="117"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="117"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="117"/>
+      <c r="B96" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="C96" s="167"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="117"/>
+      <c r="B97" s="168"/>
+      <c r="C97" s="62"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="117"/>
+      <c r="B98" s="168"/>
+      <c r="C98" s="62"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="117"/>
+      <c r="B99" s="139"/>
+      <c r="C99" s="72"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="117"/>
+      <c r="B100" s="182" t="s">
+        <v>362</v>
+      </c>
+      <c r="C100" s="62"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="117"/>
+      <c r="B101" s="168"/>
+      <c r="C101" s="62"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="117"/>
+      <c r="B102" s="183" t="s">
+        <v>363</v>
+      </c>
+      <c r="C102" s="138"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="117"/>
+      <c r="B103" s="168"/>
+      <c r="C103" s="62"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="117"/>
+      <c r="B104" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="C104" s="185"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="117"/>
+      <c r="B105" s="186" t="s">
+        <v>364</v>
+      </c>
+      <c r="C105" s="185"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="117"/>
+      <c r="B106" s="187"/>
+      <c r="C106" s="185"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="117"/>
+      <c r="B107" s="189" t="s">
+        <v>365</v>
+      </c>
+      <c r="C107" s="185"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="117"/>
+      <c r="B108" s="192" t="s">
+        <v>366</v>
+      </c>
+      <c r="C108" s="193"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="117"/>
+      <c r="B109" s="187" t="s">
+        <v>359</v>
+      </c>
+      <c r="C109" s="185"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="117"/>
+      <c r="B110" s="190" t="s">
+        <v>367</v>
+      </c>
+      <c r="C110" s="185"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="117"/>
+      <c r="B111" s="191" t="s">
+        <v>368</v>
+      </c>
+      <c r="C111" s="122"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="117"/>
+      <c r="B112" s="117"/>
+      <c r="C112" s="117"/>
+    </row>
+    <row r="118">
+      <c r="B118" s="117"/>
+      <c r="C118" s="117"/>
+      <c r="D118" s="117"/>
+    </row>
+    <row r="119">
+      <c r="B119" s="117"/>
+      <c r="C119" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="D119" s="167"/>
+    </row>
+    <row r="120">
+      <c r="B120" s="117"/>
+      <c r="C120" s="168"/>
+      <c r="D120" s="62"/>
+    </row>
+    <row r="121">
+      <c r="B121" s="117"/>
+      <c r="C121" s="168"/>
+      <c r="D121" s="62"/>
+    </row>
+    <row r="122">
+      <c r="B122" s="117"/>
+      <c r="C122" s="139"/>
+      <c r="D122" s="72"/>
+    </row>
+    <row r="123">
+      <c r="B123" s="117"/>
+      <c r="C123" s="182" t="s">
+        <v>369</v>
+      </c>
+      <c r="D123" s="62"/>
+    </row>
+    <row r="124">
+      <c r="B124" s="117"/>
+      <c r="C124" s="168"/>
+      <c r="D124" s="62"/>
+    </row>
+    <row r="125">
+      <c r="B125" s="117"/>
+      <c r="C125" s="183" t="s">
+        <v>370</v>
+      </c>
+      <c r="D125" s="138"/>
+    </row>
+    <row r="126">
+      <c r="B126" s="117"/>
+      <c r="C126" s="168"/>
+      <c r="D126" s="62"/>
+    </row>
+    <row r="127">
+      <c r="B127" s="117"/>
+      <c r="C127" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="D127" s="185"/>
+    </row>
+    <row r="128">
+      <c r="B128" s="117"/>
+      <c r="C128" s="186" t="s">
+        <v>371</v>
+      </c>
+      <c r="D128" s="185"/>
+    </row>
+    <row r="129">
+      <c r="B129" s="117"/>
+      <c r="C129" s="187"/>
+      <c r="D129" s="185"/>
+    </row>
+    <row r="130">
+      <c r="B130" s="117"/>
+      <c r="C130" s="189" t="s">
+        <v>365</v>
+      </c>
+      <c r="D130" s="185"/>
+    </row>
+    <row r="131">
+      <c r="B131" s="117"/>
+      <c r="C131" s="192" t="s">
+        <v>372</v>
+      </c>
+      <c r="D131" s="193"/>
+    </row>
+    <row r="132">
+      <c r="B132" s="117"/>
+      <c r="C132" s="187" t="s">
+        <v>359</v>
+      </c>
+      <c r="D132" s="185"/>
+    </row>
+    <row r="133">
+      <c r="B133" s="117"/>
+      <c r="C133" s="190" t="s">
+        <v>373</v>
+      </c>
+      <c r="D133" s="185"/>
+    </row>
+    <row r="134">
+      <c r="B134" s="117"/>
+      <c r="C134" s="191" t="s">
+        <v>374</v>
+      </c>
+      <c r="D134" s="122"/>
+    </row>
+    <row r="135">
+      <c r="B135" s="117"/>
+      <c r="C135" s="117"/>
+      <c r="D135" s="117"/>
+    </row>
+    <row r="143">
+      <c r="B143" s="117"/>
+      <c r="C143" s="117"/>
+      <c r="D143" s="117"/>
+    </row>
+    <row r="144">
+      <c r="B144" s="117"/>
+      <c r="C144" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="D144" s="167"/>
+    </row>
+    <row r="145">
+      <c r="B145" s="117"/>
+      <c r="C145" s="168"/>
+      <c r="D145" s="62"/>
+    </row>
+    <row r="146">
+      <c r="B146" s="117"/>
+      <c r="C146" s="168"/>
+      <c r="D146" s="62"/>
+    </row>
+    <row r="147">
+      <c r="B147" s="117"/>
+      <c r="C147" s="139"/>
+      <c r="D147" s="72"/>
+    </row>
+    <row r="148">
+      <c r="B148" s="117"/>
+      <c r="C148" s="182" t="s">
+        <v>375</v>
+      </c>
+      <c r="D148" s="62"/>
+    </row>
+    <row r="149">
+      <c r="B149" s="117"/>
+      <c r="C149" s="168"/>
+      <c r="D149" s="62"/>
+    </row>
+    <row r="150">
+      <c r="B150" s="117"/>
+      <c r="C150" s="183" t="s">
+        <v>376</v>
+      </c>
+      <c r="D150" s="138"/>
+    </row>
+    <row r="151">
+      <c r="B151" s="117"/>
+      <c r="C151" s="168"/>
+      <c r="D151" s="62"/>
+    </row>
+    <row r="152">
+      <c r="B152" s="117"/>
+      <c r="C152" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="D152" s="185"/>
+    </row>
+    <row r="153">
+      <c r="B153" s="117"/>
+      <c r="C153" s="186" t="s">
+        <v>377</v>
+      </c>
+      <c r="D153" s="185"/>
+    </row>
+    <row r="154">
+      <c r="B154" s="117"/>
+      <c r="C154" s="187"/>
+      <c r="D154" s="185"/>
+    </row>
+    <row r="155">
+      <c r="B155" s="117"/>
+      <c r="C155" s="189" t="s">
+        <v>365</v>
+      </c>
+      <c r="D155" s="185"/>
+    </row>
+    <row r="156">
+      <c r="B156" s="117"/>
+      <c r="C156" s="192" t="s">
+        <v>378</v>
+      </c>
+      <c r="D156" s="193"/>
+    </row>
+    <row r="157">
+      <c r="B157" s="117"/>
+      <c r="C157" s="187" t="s">
+        <v>359</v>
+      </c>
+      <c r="D157" s="185"/>
+    </row>
+    <row r="158">
+      <c r="B158" s="117"/>
+      <c r="C158" s="190" t="s">
+        <v>379</v>
+      </c>
+      <c r="D158" s="185"/>
+    </row>
+    <row r="159">
+      <c r="B159" s="117"/>
+      <c r="C159" s="191" t="s">
+        <v>380</v>
+      </c>
+      <c r="D159" s="122"/>
+    </row>
+    <row r="160">
+      <c r="B160" s="117"/>
+      <c r="C160" s="117"/>
+      <c r="D160" s="117"/>
+    </row>
+    <row r="166">
+      <c r="B166" s="117"/>
+      <c r="C166" s="117"/>
+      <c r="D166" s="117"/>
+    </row>
+    <row r="167">
+      <c r="B167" s="117"/>
+      <c r="C167" s="181" t="s">
+        <v>330</v>
+      </c>
+      <c r="D167" s="167"/>
+    </row>
+    <row r="168">
+      <c r="B168" s="117"/>
+      <c r="C168" s="168"/>
+      <c r="D168" s="62"/>
+    </row>
+    <row r="169">
+      <c r="B169" s="117"/>
+      <c r="C169" s="168"/>
+      <c r="D169" s="62"/>
+    </row>
+    <row r="170">
+      <c r="B170" s="117"/>
+      <c r="C170" s="139"/>
+      <c r="D170" s="72"/>
+    </row>
+    <row r="171">
+      <c r="B171" s="117"/>
+      <c r="C171" s="182" t="s">
+        <v>381</v>
+      </c>
+      <c r="D171" s="62"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="117"/>
+      <c r="C172" s="168"/>
+      <c r="D172" s="62"/>
+    </row>
+    <row r="173">
+      <c r="B173" s="117"/>
+      <c r="C173" s="183" t="s">
+        <v>382</v>
+      </c>
+      <c r="D173" s="138"/>
+    </row>
+    <row r="174">
+      <c r="B174" s="117"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="62"/>
+    </row>
+    <row r="175">
+      <c r="B175" s="117"/>
+      <c r="C175" s="184" t="s">
+        <v>333</v>
+      </c>
+      <c r="D175" s="185"/>
+    </row>
+    <row r="176">
+      <c r="B176" s="117"/>
+      <c r="C176" s="186" t="s">
+        <v>383</v>
+      </c>
+      <c r="D176" s="185"/>
+    </row>
+    <row r="177">
+      <c r="B177" s="117"/>
+      <c r="C177" s="187"/>
+      <c r="D177" s="185"/>
+    </row>
+    <row r="178">
+      <c r="B178" s="117"/>
+      <c r="C178" s="189" t="s">
+        <v>365</v>
+      </c>
+      <c r="D178" s="185"/>
+    </row>
+    <row r="179">
+      <c r="B179" s="117"/>
+      <c r="C179" s="192" t="s">
+        <v>384</v>
+      </c>
+      <c r="D179" s="193"/>
+    </row>
+    <row r="180">
+      <c r="B180" s="117"/>
+      <c r="C180" s="187" t="s">
+        <v>359</v>
+      </c>
+      <c r="D180" s="185"/>
+    </row>
+    <row r="181">
+      <c r="B181" s="117"/>
+      <c r="C181" s="190" t="s">
+        <v>385</v>
+      </c>
+      <c r="D181" s="185"/>
+    </row>
+    <row r="182">
+      <c r="B182" s="117"/>
+      <c r="C182" s="191" t="s">
+        <v>386</v>
+      </c>
+      <c r="D182" s="122"/>
+    </row>
+    <row r="183">
+      <c r="B183" s="117"/>
+      <c r="C183" s="117"/>
+      <c r="D183" s="117"/>
+    </row>
+  </sheetData>
+  <mergeCells count="81">
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="C119:D122"/>
+    <mergeCell ref="C123:D124"/>
+    <mergeCell ref="C125:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C144:D147"/>
+    <mergeCell ref="C148:D149"/>
+    <mergeCell ref="C150:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C178:D178"/>
+    <mergeCell ref="C180:D180"/>
+    <mergeCell ref="C181:D181"/>
+    <mergeCell ref="C182:D182"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="C167:D170"/>
+    <mergeCell ref="C171:D172"/>
+    <mergeCell ref="C173:D174"/>
+    <mergeCell ref="C175:D175"/>
+    <mergeCell ref="C176:D176"/>
+    <mergeCell ref="C177:D177"/>
+    <mergeCell ref="B2:C5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="C25:D28"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B50:C53"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="B56:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="C73:D76"/>
+    <mergeCell ref="C77:D78"/>
+    <mergeCell ref="C79:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="B96:C99"/>
+    <mergeCell ref="B100:C101"/>
+    <mergeCell ref="B102:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B109:C109"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B16"/>
+    <hyperlink r:id="rId2" ref="C39"/>
+    <hyperlink r:id="rId3" ref="B64"/>
+    <hyperlink r:id="rId4" ref="C87"/>
+    <hyperlink r:id="rId5" ref="B110"/>
+    <hyperlink r:id="rId6" ref="C133"/>
+    <hyperlink r:id="rId7" ref="C158"/>
+    <hyperlink r:id="rId8" ref="C181"/>
+  </hyperlinks>
+  <drawing r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>